<commit_message>
Updates to 5-11 report
</commit_message>
<xml_diff>
--- a/EC/Train Runs 2016-05-11 (FRA Format).xlsx
+++ b/EC/Train Runs 2016-05-11 (FRA Format).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860" tabRatio="845" firstSheet="5" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="13860" tabRatio="845" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Summary" sheetId="15" r:id="rId1"/>
@@ -5744,9 +5744,6 @@
     <t>4019/4164</t>
   </si>
   <si>
-    <t>Onboard logs and messaging logs do not indicate any issue. Was this cut out due to operational issues?</t>
-  </si>
-  <si>
     <t>Dispatcher training - couldn't initialize at DUS due to clearance number problems. Ran ATC until 38th (initialized there) to keep schedule</t>
   </si>
   <si>
@@ -5757,6 +5754,9 @@
   </si>
   <si>
     <t>DUS Equipment Failure.</t>
+  </si>
+  <si>
+    <t>after reviewing Onboard, Comms and DTO service logs no issues were found to explain the cutout at Peoria. Only remaing conclusing is operational.</t>
   </si>
 </sst>
 </file>
@@ -22092,8 +22092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23271,7 +23271,7 @@
         <v>2.8541666666569654E-2</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>1813</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -24134,7 +24134,7 @@
         <v>2.2395833337213844E-2</v>
       </c>
       <c r="G89" s="19" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -24766,7 +24766,7 @@
         <v>2.8217592596774921E-2</v>
       </c>
       <c r="G119" s="19" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="120" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -25346,7 +25346,7 @@
         <v>2.4201388885558117E-2</v>
       </c>
       <c r="G146" s="19" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="H146"/>
       <c r="L146"/>
@@ -26393,8 +26393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F103"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26505,7 +26505,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="77" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="C13" s="79">
         <f>$C$99</f>

</xml_diff>